<commit_message>
Upload: -PGM homework 5 bookwork and EM algorithm results as well as code for EM algorithm.
</commit_message>
<xml_diff>
--- a/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
+++ b/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -88,13 +88,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,58 +159,59 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
-                <c:formatCode>0.00000E+00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.4331325192982998E-16</c:v>
+                  <c:v>762957.95475691999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1497446272771599E-16</c:v>
+                  <c:v>229725.89961944899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3627226029913601E-16</c:v>
+                  <c:v>59192.511157275803</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7381251013103297E-17</c:v>
+                  <c:v>18436.239720580299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6346098896209101E-17</c:v>
+                  <c:v>6450.4833894153599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showVal val="1"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="48030464"/>
-        <c:axId val="48032000"/>
+        <c:axId val="59873920"/>
+        <c:axId val="62304640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48030464"/>
+        <c:axId val="59873920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48032000"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="62304640"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48032000"/>
+        <c:axId val="62304640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="48030464"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59873920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -219,7 +220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -548,71 +549,72 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>3.4331325192982998E-16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3.1497446272771599E-16</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.3627226029913601E-16</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4.7381251013103297E-17</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.6346098896209101E-17</v>
+      <c r="B2" s="3">
+        <v>762957.95475691999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>229725.89961944899</v>
+      </c>
+      <c r="D2" s="3">
+        <v>59192.511157275803</v>
+      </c>
+      <c r="E2" s="3">
+        <v>18436.239720580299</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6450.4833894153599</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Upload: -PGM homework 5 now includes Chow-liu structure learning. -Some results for some runs.
Note: EM algorithm is bork (M step produces uniform functions almost always). WeightedEdgeComparator.java violates its promises when used with Collections.sort() extremely rarely and breaks a couple runs.
</commit_message>
<xml_diff>
--- a/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
+++ b/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="1.uai" sheetId="1" r:id="rId1"/>
+    <sheet name="2.uai" sheetId="2" r:id="rId2"/>
+    <sheet name="3.uai" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>BN_MLE_FOD</t>
   </si>
@@ -47,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -94,7 +94,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,7 +120,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>'1.uai'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -134,7 +134,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'1.uai'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -157,7 +157,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>'1.uai'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -181,29 +181,28 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="59873920"/>
-        <c:axId val="62304640"/>
+        <c:axId val="60791424"/>
+        <c:axId val="64729472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59873920"/>
+        <c:axId val="60791424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62304640"/>
+        <c:crossAx val="64729472"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62304640"/>
+        <c:axId val="64729472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -211,7 +210,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59873920"/>
+        <c:crossAx val="60791424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -220,8 +219,988 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.uai'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BN_EM_POD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.uai'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>280141085.54763699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>314442202.85992801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>303348476.09609997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="88833408"/>
+        <c:axId val="61928192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88833408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61928192"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61928192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88833408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.uai'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BS_CL_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.uai'!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2391694.3153721602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>626756.28291258798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>339444.99837692699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>329758.15310405102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="61823232"/>
+        <c:axId val="61874944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="61823232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61874944"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61874944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61823232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2.uai'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BN_MLE_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.uai'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>849611.67438366404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>553423.84143398097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>234249.70695535099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61973.028773906401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14481.1527033107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="66070784"/>
+        <c:axId val="66077440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="66070784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66077440"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66077440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66070784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2.uai'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BN_MLE_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.uai'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>849611.67438366404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>553423.84143398097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>234249.70695535099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61973.028773906401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14481.1527033107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="61842560"/>
+        <c:axId val="67320832"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="61842560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67320832"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="67320832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61842560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2.uai'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BS_CL_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.uai'!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>510457.04181706498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137924.40155050199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28066.4993748136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="67762816"/>
+        <c:axId val="69575040"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="67762816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69575040"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69575040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67762816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16251829998822706"/>
+          <c:y val="0.19480351414406533"/>
+          <c:w val="0.78876469709578978"/>
+          <c:h val="0.69384623797025369"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3.uai'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BN_MLE_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.uai'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5645670.08072583</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>863624.13064619596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94328.636518277301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18915.552091688201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5583.8769811004904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="88887680"/>
+        <c:axId val="88889216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88887680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88889216"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88889216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88887680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16251829998822712"/>
+          <c:y val="0.19480351414406533"/>
+          <c:w val="0.78876469709579"/>
+          <c:h val="0.69384623797025369"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3.uai'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BN_MLE_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.uai'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5645670.08072583</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>863624.13064619596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94328.636518277301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18915.552091688201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5583.8769811004904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="70394240"/>
+        <c:axId val="73388032"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70394240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73388032"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73388032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70394240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16251829998822712"/>
+          <c:y val="0.19480351414406533"/>
+          <c:w val="0.78876469709579"/>
+          <c:h val="0.69384623797025369"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3.uai'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BS_CL_FOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3.uai'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Train-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Train-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Train-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Train-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Train-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.uai'!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13545385.9022338</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3254763.1508173998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2371640.5395453302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2328699.81227468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="88901888"/>
+        <c:axId val="88425600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88901888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88425600"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88425600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88901888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -231,15 +1210,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>123826</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742951</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -253,6 +1232,256 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>714376</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -548,14 +1777,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>762957.95475691999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>229725.89961944899</v>
+      </c>
+      <c r="D2" s="3">
+        <v>59192.511157275803</v>
+      </c>
+      <c r="E2" s="3">
+        <v>18436.239720580299</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6450.4833894153599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>280141085.54763699</v>
+      </c>
+      <c r="C3" s="3">
+        <v>314442202.85992801</v>
+      </c>
+      <c r="D3" s="3">
+        <v>303348476.09609997</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2391694.3153721602</v>
+      </c>
+      <c r="C4" s="3">
+        <v>626756.28291258798</v>
+      </c>
+      <c r="D4" s="3">
+        <v>339444.99837692699</v>
+      </c>
+      <c r="E4" s="3">
+        <v>329758.15310405102</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -581,26 +1904,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>762957.95475691999</v>
+        <v>849611.67438366404</v>
       </c>
       <c r="C2" s="3">
-        <v>229725.89961944899</v>
+        <v>553423.84143398097</v>
       </c>
       <c r="D2" s="3">
-        <v>59192.511157275803</v>
+        <v>234249.70695535099</v>
       </c>
       <c r="E2" s="3">
-        <v>18436.239720580299</v>
+        <v>61973.028773906401</v>
       </c>
       <c r="F2" s="3">
-        <v>6450.4833894153599</v>
+        <v>14481.1527033107</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>299825670.14754897</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -610,39 +1935,110 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="3">
+        <v>510457.04181706498</v>
+      </c>
+      <c r="C4" s="3">
+        <v>137924.40155050199</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>28066.4993748136</v>
+      </c>
       <c r="F4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5645670.08072583</v>
+      </c>
+      <c r="C2" s="3">
+        <v>863624.13064619596</v>
+      </c>
+      <c r="D2" s="3">
+        <v>94328.636518277301</v>
+      </c>
+      <c r="E2" s="3">
+        <v>18915.552091688201</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5583.8769811004904</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>299825670.14754897</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>13545385.9022338</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3254763.1508173998</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2371640.5395453302</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2328699.81227468</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Upload: -Finished PGM homework5. Not all runs completed. Still some wonky error with "comparator violates its general contract" on extremely rare occasions.
</commit_message>
<xml_diff>
--- a/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
+++ b/projects/graduate/cs6301-probabilistic-graphical-models/homework5/output/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="1.uai" sheetId="1" r:id="rId1"/>
@@ -184,25 +184,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="60791424"/>
-        <c:axId val="64729472"/>
+        <c:axId val="84978304"/>
+        <c:axId val="96526720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60791424"/>
+        <c:axId val="84978304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64729472"/>
+        <c:crossAx val="96526720"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64729472"/>
+        <c:axId val="96526720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -210,7 +210,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60791424"/>
+        <c:crossAx val="84978304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -219,7 +219,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -291,6 +291,9 @@
                 <c:pt idx="2">
                   <c:v>303348476.09609997</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>280140818.98002499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -299,25 +302,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="88833408"/>
-        <c:axId val="61928192"/>
+        <c:axId val="96608256"/>
+        <c:axId val="96609792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88833408"/>
+        <c:axId val="96608256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61928192"/>
+        <c:crossAx val="96609792"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61928192"/>
+        <c:axId val="96609792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -325,7 +328,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88833408"/>
+        <c:crossAx val="96608256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -334,7 +337,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -417,25 +420,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="61823232"/>
-        <c:axId val="61874944"/>
+        <c:axId val="96638080"/>
+        <c:axId val="96639616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61823232"/>
+        <c:axId val="96638080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61874944"/>
+        <c:crossAx val="96639616"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61874944"/>
+        <c:axId val="96639616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +446,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61823232"/>
+        <c:crossAx val="96638080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -452,7 +455,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -538,25 +541,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="66070784"/>
-        <c:axId val="66077440"/>
+        <c:axId val="96676480"/>
+        <c:axId val="96698752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66070784"/>
+        <c:axId val="96676480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66077440"/>
+        <c:crossAx val="96698752"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66077440"/>
+        <c:axId val="96698752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +567,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66070784"/>
+        <c:crossAx val="96676480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -573,7 +576,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -595,11 +598,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2.uai'!$A$2</c:f>
+              <c:f>'2.uai'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BN_MLE_FOD</c:v>
+                  <c:v>BN_EM_POD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -632,24 +635,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2.uai'!$B$2:$F$2</c:f>
+              <c:f>'2.uai'!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>849611.67438366404</c:v>
+                  <c:v>299825670.14754897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>553423.84143398097</c:v>
+                  <c:v>147675298.55651101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>234249.70695535099</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>61973.028773906401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14481.1527033107</c:v>
+                  <c:v>116308480.221587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -659,25 +656,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="61842560"/>
-        <c:axId val="67320832"/>
+        <c:axId val="96718848"/>
+        <c:axId val="96720384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61842560"/>
+        <c:axId val="96718848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67320832"/>
+        <c:crossAx val="96720384"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67320832"/>
+        <c:axId val="96720384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +682,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61842560"/>
+        <c:crossAx val="96718848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -694,7 +691,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -774,25 +771,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="67762816"/>
-        <c:axId val="69575040"/>
+        <c:axId val="97342592"/>
+        <c:axId val="97344128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67762816"/>
+        <c:axId val="97342592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69575040"/>
+        <c:crossAx val="97344128"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69575040"/>
+        <c:axId val="97344128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +797,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67762816"/>
+        <c:crossAx val="97342592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -809,7 +806,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -828,9 +825,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16251829998822706"/>
+          <c:x val="0.16251829998822709"/>
           <c:y val="0.19480351414406533"/>
-          <c:w val="0.78876469709578978"/>
+          <c:w val="0.78876469709578989"/>
           <c:h val="0.69384623797025369"/>
         </c:manualLayout>
       </c:layout>
@@ -905,25 +902,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="88887680"/>
-        <c:axId val="88889216"/>
+        <c:axId val="97478912"/>
+        <c:axId val="97497088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88887680"/>
+        <c:axId val="97478912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88889216"/>
+        <c:crossAx val="97497088"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88889216"/>
+        <c:axId val="97497088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +928,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88887680"/>
+        <c:crossAx val="97478912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,7 +937,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -959,9 +956,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16251829998822712"/>
+          <c:x val="0.16251829998822717"/>
           <c:y val="0.19480351414406533"/>
-          <c:w val="0.78876469709579"/>
+          <c:w val="0.78876469709579011"/>
           <c:h val="0.69384623797025369"/>
         </c:manualLayout>
       </c:layout>
@@ -972,11 +969,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3.uai'!$A$2</c:f>
+              <c:f>'3.uai'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BN_MLE_FOD</c:v>
+                  <c:v>BN_EM_POD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1009,24 +1006,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3.uai'!$B$2:$F$2</c:f>
+              <c:f>'3.uai'!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5645670.08072583</c:v>
+                  <c:v>15844404.535230299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>863624.13064619596</c:v>
+                  <c:v>15844404.535230299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>94328.636518277301</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18915.552091688201</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5583.8769811004904</c:v>
+                  <c:v>15844404.535230299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1036,25 +1027,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="70394240"/>
-        <c:axId val="73388032"/>
+        <c:axId val="97602944"/>
+        <c:axId val="97604736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70394240"/>
+        <c:axId val="97602944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73388032"/>
+        <c:crossAx val="97604736"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73388032"/>
+        <c:axId val="97604736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1062,7 +1053,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70394240"/>
+        <c:crossAx val="97602944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1071,7 +1062,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1090,9 +1081,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16251829998822712"/>
+          <c:x val="0.16251829998822717"/>
           <c:y val="0.19480351414406533"/>
-          <c:w val="0.78876469709579"/>
+          <c:w val="0.78876469709579011"/>
           <c:h val="0.69384623797025369"/>
         </c:manualLayout>
       </c:layout>
@@ -1164,25 +1155,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="88901888"/>
-        <c:axId val="88425600"/>
+        <c:axId val="97628928"/>
+        <c:axId val="97630464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88901888"/>
+        <c:axId val="97628928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88425600"/>
+        <c:crossAx val="97630464"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88425600"/>
+        <c:axId val="97630464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1181,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88901888"/>
+        <c:crossAx val="97628928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1199,7 +1190,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1777,15 +1768,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1838,7 +1829,9 @@
       <c r="D3" s="3">
         <v>303348476.09609997</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>280140818.98002499</v>
+      </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
@@ -1870,16 +1863,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1926,8 +1918,12 @@
       <c r="B3" s="3">
         <v>299825670.14754897</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3">
+        <v>147675298.55651101</v>
+      </c>
+      <c r="D3" s="3">
+        <v>116308480.221587</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
@@ -1958,16 +1954,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2012,10 +2008,14 @@
         <v>6</v>
       </c>
       <c r="B3" s="3">
-        <v>299825670.14754897</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+        <v>15844404.535230299</v>
+      </c>
+      <c r="C3" s="3">
+        <v>15844404.535230299</v>
+      </c>
+      <c r="D3" s="3">
+        <v>15844404.535230299</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>

</xml_diff>